<commit_message>
Storing type for variables
</commit_message>
<xml_diff>
--- a/data/forsk_termer.xlsx
+++ b/data/forsk_termer.xlsx
@@ -15,29 +15,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="281">
   <si>
     <t>Forskningsbiblioteken</t>
   </si>
   <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>VariableType</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
     <t>forsk1</t>
   </si>
   <si>
     <t>Organisationsnamn</t>
   </si>
   <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>xsd:string</t>
+  </si>
+  <si>
     <t>forsk2</t>
   </si>
   <si>
     <t>Respondent-ID i gammal databas</t>
   </si>
   <si>
+    <t>xsd:integer</t>
+  </si>
+  <si>
     <t>forsk3</t>
   </si>
   <si>
     <t>Årsverken Bibliotekarier och dokumentalister; Kvinnor</t>
   </si>
   <si>
+    <t>xsd:decimal</t>
+  </si>
+  <si>
     <t>forsk4</t>
   </si>
   <si>
@@ -779,7 +803,7 @@
     <t>forsk127</t>
   </si>
   <si>
-    <t>Antal biblioteksanställda som arbetade med formell lärarledd undervisning </t>
+    <t>Antal biblioteksanställda som arbetade med formell lärarledd undervisning</t>
   </si>
   <si>
     <t>forsk128</t>
@@ -791,7 +815,7 @@
     <t>forsk129</t>
   </si>
   <si>
-    <t>Antal virtuella besök av IP-besökare på digitala pedagogiska resurser </t>
+    <t>Antal virtuella besök av IP-besökare på digitala pedagogiska resurser</t>
   </si>
   <si>
     <t>forsk130</t>
@@ -815,7 +839,7 @@
     <t>forsk133</t>
   </si>
   <si>
-    <t>Antal poster som indexerats av biblioteket i databaser och andra informationstjänster. </t>
+    <t>Antal poster som indexerats av biblioteket i databaser och andra informationstjänster.</t>
   </si>
   <si>
     <t>forsk134</t>
@@ -844,11 +868,12 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -880,6 +905,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -890,14 +922,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD7E4BD"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FFD7E4BD"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -935,8 +967,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -944,15 +984,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1041,1110 +1089,1911 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B137"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A111" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E138" activeCellId="0" sqref="E138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="88.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="88.2142857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>40</v>
+      <c r="A21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>42</v>
+      <c r="A22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>44</v>
+      <c r="A23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>46</v>
+      <c r="A24" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>48</v>
+      <c r="A25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>50</v>
+      <c r="A26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>52</v>
+      <c r="A27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>54</v>
+      <c r="A28" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>56</v>
+      <c r="A29" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>58</v>
+      <c r="A30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>60</v>
+      <c r="A31" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>62</v>
+      <c r="A32" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>64</v>
+      <c r="A33" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>66</v>
+      <c r="A34" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>68</v>
+      <c r="A35" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>70</v>
+      <c r="A36" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>72</v>
+      <c r="A37" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>74</v>
+      <c r="A38" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>76</v>
+      <c r="A39" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>78</v>
+      <c r="A40" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>80</v>
+      <c r="A41" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>82</v>
+      <c r="A42" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>84</v>
+      <c r="A43" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>86</v>
+      <c r="A44" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>88</v>
+      <c r="A45" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>90</v>
+      <c r="A46" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>92</v>
+      <c r="A47" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>94</v>
+      <c r="A48" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>96</v>
+      <c r="A49" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>98</v>
+      <c r="A50" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>100</v>
+      <c r="A51" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>102</v>
+      <c r="A52" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>104</v>
+      <c r="A53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>106</v>
+      <c r="A54" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>108</v>
+      <c r="A55" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>110</v>
+      <c r="A56" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>112</v>
+      <c r="A57" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>114</v>
+      <c r="A58" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>116</v>
+      <c r="A59" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>118</v>
+      <c r="A60" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>120</v>
+      <c r="A61" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>122</v>
+      <c r="A62" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>124</v>
+      <c r="A63" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>126</v>
+      <c r="A64" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>128</v>
+      <c r="A65" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>130</v>
+      <c r="A66" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>132</v>
+      <c r="A67" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>134</v>
+      <c r="A68" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>136</v>
+      <c r="A69" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>138</v>
+      <c r="A70" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>140</v>
+      <c r="A71" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>142</v>
+      <c r="A72" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>144</v>
+      <c r="A73" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>146</v>
+      <c r="A74" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>148</v>
+      <c r="A75" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>150</v>
+      <c r="A76" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>152</v>
+      <c r="A77" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>154</v>
+      <c r="A78" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>156</v>
+      <c r="A79" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>158</v>
+      <c r="A80" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>160</v>
+      <c r="A81" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>162</v>
+      <c r="A82" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>164</v>
+      <c r="A83" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>166</v>
+      <c r="A84" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>168</v>
+      <c r="A85" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>170</v>
+      <c r="A86" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>172</v>
+      <c r="A87" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>174</v>
+      <c r="A88" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>176</v>
+      <c r="A89" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>178</v>
+      <c r="A90" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>180</v>
+      <c r="A91" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>182</v>
+      <c r="A92" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>184</v>
+      <c r="A93" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>186</v>
+      <c r="A94" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>188</v>
+      <c r="A95" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>190</v>
+      <c r="A96" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>192</v>
+      <c r="A97" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>194</v>
+      <c r="A98" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>196</v>
+      <c r="A99" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>198</v>
+      <c r="A100" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>200</v>
+      <c r="A101" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>202</v>
+      <c r="A102" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>204</v>
+      <c r="A103" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>206</v>
+      <c r="A104" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>208</v>
+      <c r="A105" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>210</v>
+      <c r="A106" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>212</v>
+      <c r="A107" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>214</v>
+      <c r="A108" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>216</v>
+      <c r="A109" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>218</v>
+      <c r="A110" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>220</v>
+      <c r="A111" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>222</v>
+      <c r="A112" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>224</v>
+      <c r="A113" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>226</v>
+      <c r="A114" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>228</v>
+      <c r="A115" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>230</v>
+      <c r="A116" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>232</v>
+      <c r="A117" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>234</v>
+      <c r="A118" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>236</v>
+      <c r="A119" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>238</v>
+      <c r="A120" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>240</v>
+      <c r="A121" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>242</v>
+      <c r="A122" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>244</v>
+      <c r="A123" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>246</v>
+      <c r="A124" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>248</v>
+      <c r="A125" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>250</v>
+      <c r="A126" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>252</v>
+      <c r="A127" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>254</v>
+      <c r="A128" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>256</v>
+      <c r="A129" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>258</v>
+      <c r="A130" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>260</v>
+      <c r="A131" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>262</v>
+      <c r="A132" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>264</v>
+      <c r="A133" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>266</v>
+      <c r="A134" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>268</v>
+      <c r="A135" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>270</v>
+      <c r="A136" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>272</v>
+      <c r="A137" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Library name, municipality and county should not be public fields
</commit_message>
<xml_diff>
--- a/data/forsk_termer.xlsx
+++ b/data/forsk_termer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="281">
   <si>
     <t>Forskningsbiblioteken</t>
   </si>
@@ -38,25 +38,25 @@
     <t>Organisationsnamn</t>
   </si>
   <si>
+    <t>xsd:string</t>
+  </si>
+  <si>
+    <t>forsk2</t>
+  </si>
+  <si>
+    <t>Respondent-ID i gammal databas</t>
+  </si>
+  <si>
+    <t>xsd:integer</t>
+  </si>
+  <si>
+    <t>forsk3</t>
+  </si>
+  <si>
+    <t>Årsverken Bibliotekarier och dokumentalister; Kvinnor</t>
+  </si>
+  <si>
     <t>public</t>
-  </si>
-  <si>
-    <t>xsd:string</t>
-  </si>
-  <si>
-    <t>forsk2</t>
-  </si>
-  <si>
-    <t>Respondent-ID i gammal databas</t>
-  </si>
-  <si>
-    <t>xsd:integer</t>
-  </si>
-  <si>
-    <t>forsk3</t>
-  </si>
-  <si>
-    <t>Årsverken Bibliotekarier och dokumentalister; Kvinnor</t>
   </si>
   <si>
     <t>xsd:decimal</t>
@@ -976,10 +976,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1006,6 +1002,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1091,1909 +1091,1913 @@
   </sheetPr>
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A111" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E138" activeCellId="0" sqref="E138"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6785714285714"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="88.2142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.2602040816327"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="4" t="s">
+    <row r="1" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="D3" s="0"/>
       <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
+      <c r="D4" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
+      <c r="D5" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
+      <c r="D6" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
+      <c r="D7" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
+      <c r="D8" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
+      <c r="D9" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
+      <c r="D10" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
+      <c r="D11" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>7</v>
+      <c r="D12" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>7</v>
+      <c r="D13" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
+      <c r="D14" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
+      <c r="D15" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
+      <c r="D16" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>7</v>
+      <c r="D17" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
+      <c r="D18" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>7</v>
+      <c r="D19" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="D20" s="0"/>
       <c r="E20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>7</v>
+      <c r="D21" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>7</v>
+      <c r="D22" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>7</v>
+      <c r="D23" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>53</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>7</v>
+      <c r="D24" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>7</v>
+      <c r="D25" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>7</v>
+      <c r="D26" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>7</v>
+      <c r="D27" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>7</v>
+      <c r="D28" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>7</v>
+      <c r="D29" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>7</v>
+      <c r="D30" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>7</v>
+      <c r="D31" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>7</v>
+      <c r="D32" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="D33" s="0"/>
       <c r="E33" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>7</v>
+      <c r="D34" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>7</v>
+      <c r="D35" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>7</v>
+      <c r="D36" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>7</v>
+      <c r="D37" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>7</v>
+      <c r="D38" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>7</v>
+      <c r="D39" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>7</v>
+      <c r="D40" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="7" t="s">
         <v>87</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>7</v>
+      <c r="D41" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>7</v>
+      <c r="D42" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>7</v>
+      <c r="D43" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>7</v>
+      <c r="D44" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>7</v>
+      <c r="D45" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>7</v>
+      <c r="D46" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>7</v>
+      <c r="D47" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="7" t="s">
         <v>101</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>7</v>
+      <c r="D48" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>7</v>
+      <c r="D49" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>7</v>
+      <c r="D50" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>7</v>
+      <c r="D51" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>7</v>
+      <c r="D52" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>7</v>
+      <c r="D53" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="7" t="s">
         <v>113</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>7</v>
+      <c r="D54" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>7</v>
+      <c r="D55" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>7</v>
+      <c r="D56" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>7</v>
+      <c r="D57" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="7" t="s">
         <v>121</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>7</v>
+      <c r="D58" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="7" t="s">
         <v>123</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>7</v>
+      <c r="D59" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="7" t="s">
         <v>125</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>7</v>
+      <c r="D60" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="7" t="s">
         <v>127</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>7</v>
+      <c r="D61" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="s">
+      <c r="A62" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>7</v>
+      <c r="D62" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>7</v>
+      <c r="D63" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>7</v>
+      <c r="D64" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="7" t="s">
         <v>135</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>7</v>
+      <c r="D65" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8" t="s">
+      <c r="A66" s="7" t="s">
         <v>137</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>7</v>
+      <c r="D66" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="7" t="s">
         <v>139</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>7</v>
+      <c r="D67" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="7" t="s">
         <v>141</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>7</v>
+      <c r="D68" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="8" t="s">
+      <c r="A69" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>7</v>
+      <c r="D69" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8" t="s">
+      <c r="A70" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>7</v>
+      <c r="D70" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="8" t="s">
+      <c r="A71" s="7" t="s">
         <v>147</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>7</v>
+      <c r="D71" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="8" t="s">
+      <c r="A72" s="7" t="s">
         <v>149</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>7</v>
+      <c r="D72" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="7" t="s">
         <v>151</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>7</v>
+      <c r="D73" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="7" t="s">
         <v>153</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>7</v>
+      <c r="D74" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="7" t="s">
         <v>155</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>7</v>
+      <c r="D75" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="7" t="s">
         <v>157</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>7</v>
+      <c r="D76" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="7" t="s">
         <v>159</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>160</v>
       </c>
+      <c r="D77" s="0"/>
       <c r="E77" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="7" t="s">
         <v>161</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="D78" s="0"/>
       <c r="E78" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="7" t="s">
         <v>163</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>7</v>
+      <c r="D79" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="7" t="s">
         <v>165</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>7</v>
+      <c r="D80" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="7" t="s">
         <v>167</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>7</v>
+      <c r="D81" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="7" t="s">
         <v>169</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>7</v>
+      <c r="D82" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="7" t="s">
         <v>171</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>7</v>
+      <c r="D83" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="7" t="s">
         <v>173</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>7</v>
+      <c r="D84" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="7" t="s">
         <v>175</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>7</v>
+      <c r="D85" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="7" t="s">
         <v>177</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>7</v>
+      <c r="D86" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="8" t="s">
+      <c r="A87" s="7" t="s">
         <v>179</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>7</v>
+      <c r="D87" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="8" t="s">
+      <c r="A88" s="7" t="s">
         <v>181</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>7</v>
+      <c r="D88" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="8" t="s">
+      <c r="A89" s="7" t="s">
         <v>183</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>7</v>
+      <c r="D89" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="8" t="s">
+      <c r="A90" s="7" t="s">
         <v>185</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>7</v>
+      <c r="D90" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="8" t="s">
+      <c r="A91" s="7" t="s">
         <v>187</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D91" s="2" t="s">
-        <v>7</v>
+      <c r="D91" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="8" t="s">
+      <c r="A92" s="7" t="s">
         <v>189</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>7</v>
+      <c r="D92" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="8" t="s">
+      <c r="A93" s="7" t="s">
         <v>191</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>7</v>
+      <c r="D93" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="8" t="s">
+      <c r="A94" s="7" t="s">
         <v>193</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>7</v>
+      <c r="D94" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="8" t="s">
+      <c r="A95" s="7" t="s">
         <v>195</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D95" s="2" t="s">
-        <v>7</v>
+      <c r="D95" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="8" t="s">
+      <c r="A96" s="7" t="s">
         <v>197</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D96" s="2" t="s">
-        <v>7</v>
+      <c r="D96" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="8" t="s">
+      <c r="A97" s="7" t="s">
         <v>199</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>7</v>
+      <c r="D97" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="8" t="s">
+      <c r="A98" s="7" t="s">
         <v>201</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>7</v>
+      <c r="D98" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="8" t="s">
+      <c r="A99" s="7" t="s">
         <v>203</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>7</v>
+      <c r="D99" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="8" t="s">
+      <c r="A100" s="7" t="s">
         <v>205</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>7</v>
+      <c r="D100" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="8" t="s">
+      <c r="A101" s="7" t="s">
         <v>207</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>7</v>
+      <c r="D101" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="8" t="s">
+      <c r="A102" s="7" t="s">
         <v>209</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D102" s="2" t="s">
-        <v>7</v>
+      <c r="D102" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="8" t="s">
+      <c r="A103" s="7" t="s">
         <v>211</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D103" s="2" t="s">
-        <v>7</v>
+      <c r="D103" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="8" t="s">
+      <c r="A104" s="7" t="s">
         <v>213</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>7</v>
+      <c r="D104" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="8" t="s">
+      <c r="A105" s="7" t="s">
         <v>215</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D105" s="2" t="s">
-        <v>7</v>
+      <c r="D105" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="8" t="s">
+      <c r="A106" s="7" t="s">
         <v>217</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D106" s="2" t="s">
-        <v>7</v>
+      <c r="D106" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="8" t="s">
+      <c r="A107" s="7" t="s">
         <v>219</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D107" s="2" t="s">
-        <v>7</v>
+      <c r="D107" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="8" t="s">
+      <c r="A108" s="7" t="s">
         <v>221</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D108" s="2" t="s">
-        <v>7</v>
+      <c r="D108" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="8" t="s">
+      <c r="A109" s="7" t="s">
         <v>223</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>7</v>
+      <c r="D109" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="8" t="s">
+      <c r="A110" s="7" t="s">
         <v>225</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>7</v>
+      <c r="D110" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="8" t="s">
+      <c r="A111" s="7" t="s">
         <v>227</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>7</v>
+      <c r="D111" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="8" t="s">
+      <c r="A112" s="7" t="s">
         <v>229</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>7</v>
+      <c r="D112" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="8" t="s">
+      <c r="A113" s="7" t="s">
         <v>231</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>7</v>
+      <c r="D113" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="8" t="s">
+      <c r="A114" s="7" t="s">
         <v>233</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>7</v>
+      <c r="D114" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="8" t="s">
+      <c r="A115" s="7" t="s">
         <v>235</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>7</v>
+      <c r="D115" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="8" t="s">
+      <c r="A116" s="7" t="s">
         <v>237</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>7</v>
+      <c r="D116" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="8" t="s">
+      <c r="A117" s="7" t="s">
         <v>239</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>7</v>
+      <c r="D117" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="8" t="s">
+      <c r="A118" s="7" t="s">
         <v>241</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D118" s="2" t="s">
-        <v>7</v>
+      <c r="D118" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="8" t="s">
+      <c r="A119" s="7" t="s">
         <v>243</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>7</v>
+      <c r="D119" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="8" t="s">
+      <c r="A120" s="7" t="s">
         <v>245</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="D120" s="0"/>
       <c r="E120" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="8" t="s">
+      <c r="A121" s="7" t="s">
         <v>247</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>7</v>
+      <c r="D121" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="8" t="s">
+      <c r="A122" s="7" t="s">
         <v>249</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>7</v>
+      <c r="D122" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="8" t="s">
+      <c r="A123" s="7" t="s">
         <v>251</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>7</v>
+      <c r="D123" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="8" t="s">
+      <c r="A124" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D124" s="2" t="s">
-        <v>7</v>
+      <c r="D124" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="8" t="s">
+      <c r="A125" s="7" t="s">
         <v>255</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>256</v>
       </c>
+      <c r="D125" s="0"/>
       <c r="E125" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="8" t="s">
+      <c r="A126" s="7" t="s">
         <v>257</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="D126" s="2" t="s">
-        <v>7</v>
+      <c r="D126" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="8" t="s">
+      <c r="A127" s="7" t="s">
         <v>259</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D127" s="2" t="s">
-        <v>7</v>
+      <c r="D127" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="8" t="s">
+      <c r="A128" s="7" t="s">
         <v>261</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D128" s="2" t="s">
-        <v>7</v>
+      <c r="D128" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="8" t="s">
+      <c r="A129" s="7" t="s">
         <v>263</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D129" s="2" t="s">
-        <v>7</v>
+      <c r="D129" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="8" t="s">
+      <c r="A130" s="7" t="s">
         <v>265</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D130" s="2" t="s">
-        <v>7</v>
+      <c r="D130" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="8" t="s">
+      <c r="A131" s="7" t="s">
         <v>267</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D131" s="2" t="s">
-        <v>7</v>
+      <c r="D131" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="8" t="s">
+      <c r="A132" s="7" t="s">
         <v>269</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D132" s="2" t="s">
-        <v>7</v>
+      <c r="D132" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="8" t="s">
+      <c r="A133" s="7" t="s">
         <v>271</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D133" s="2" t="s">
-        <v>7</v>
+      <c r="D133" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="8" t="s">
+      <c r="A134" s="7" t="s">
         <v>273</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D134" s="2" t="s">
-        <v>7</v>
+      <c r="D134" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="8" t="s">
+      <c r="A135" s="7" t="s">
         <v>275</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>276</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="8" t="s">
+      <c r="A136" s="7" t="s">
         <v>277</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>278</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="8" t="s">
+      <c r="A137" s="7" t="s">
         <v>279</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>280</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>